<commit_message>
Adding cox regression analysis to AP_Plots
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caitlyn\Box\Research\air_pollution\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caitlyn\Code\R\research\bolton\UKBB-air-pollution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75F01C62-867B-4961-BFA8-003804D01FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A491FDF6-732A-47AA-9EE8-D518DFCF54F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="14010" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="codebook" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1300,11 +1300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Updated data generation column for t_lungCancer and cancerDate_Lung. Removed duplicate baselineDate variable.
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caitlyn\Code\R\research\bolton\UKBB-air-pollution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A491FDF6-732A-47AA-9EE8-D518DFCF54F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC11289-C857-4A6B-BDE1-A91BFBBE7E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="132">
   <si>
     <t xml:space="preserve">eid </t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>no2_2010per10</t>
-  </si>
-  <si>
-    <t>baselineDate</t>
   </si>
   <si>
     <t>dob</t>
@@ -426,6 +423,25 @@
   </si>
   <si>
     <t>dateCensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current smoker &gt;19 pack year,  Current smoker 1-19 pack year, Current smoker unknown pack year,
+Never smoker,
+Past smoker &gt;19 pack year,
+Past smoker 1-19 pack year,
+Past smoker unknown pack year </t>
+  </si>
+  <si>
+    <t>Caitlyn created column in solid_all_0912.csv. Duplicate eid are filtered out in the AP_data_processing.R script, making this time to first lung cancer diagnosis.</t>
+  </si>
+  <si>
+    <t>Caitlyn created column in solid_all_0912.csv. Duplicate eid are filtered out in the AP_data_processing.R script, making this date of first lung cancer diagnosis.</t>
   </si>
 </sst>
 </file>
@@ -1301,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1319,19 +1335,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1339,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1347,10 +1363,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1358,10 +1374,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -1369,16 +1385,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1386,10 +1402,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -1397,13 +1413,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -1412,13 +1428,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="5"/>
     </row>
@@ -1427,13 +1443,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -1442,13 +1458,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -1457,13 +1473,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -1472,13 +1488,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1486,13 +1502,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1500,13 +1516,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1514,13 +1530,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1528,13 +1544,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -1542,13 +1558,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -1556,13 +1572,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1570,43 +1586,43 @@
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1614,7 +1630,7 @@
         <v>18</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1622,7 +1638,7 @@
         <v>19</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1630,10 +1646,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1641,7 +1657,7 @@
         <v>21</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1649,10 +1665,10 @@
         <v>22</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1661,15 +1677,18 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="D29" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="E29" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1677,10 +1696,10 @@
         <v>25</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1688,10 +1707,13 @@
         <v>27</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1699,10 +1721,10 @@
         <v>26</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1710,10 +1732,10 @@
         <v>28</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1721,10 +1743,10 @@
         <v>29</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1732,10 +1754,10 @@
         <v>31</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1743,10 +1765,10 @@
         <v>32</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1754,10 +1776,10 @@
         <v>33</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1765,10 +1787,10 @@
         <v>30</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1776,15 +1798,18 @@
         <v>34</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>117</v>
+      <c r="D40" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1792,7 +1817,7 @@
         <v>36</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1800,7 +1825,7 @@
         <v>37</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1808,7 +1833,7 @@
         <v>38</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1816,7 +1841,7 @@
         <v>39</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1824,68 +1849,65 @@
         <v>40</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E46" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>50</v>
+        <v>123</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>113</v>
+        <v>57</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="E51" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>